<commit_message>
Added the API to git hub and updated the dev journal for this week.
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="7740"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>DoorState</t>
   </si>
@@ -43,13 +43,43 @@
   </si>
   <si>
     <t>What it Does</t>
+  </si>
+  <si>
+    <t>Vacant?</t>
+  </si>
+  <si>
+    <t>Vacant</t>
+  </si>
+  <si>
+    <t>Occupied</t>
+  </si>
+  <si>
+    <t>Occupants</t>
+  </si>
+  <si>
+    <t>Everytime sensor 1 then sensor 2 add 1 and subtract for opposite</t>
+  </si>
+  <si>
+    <t>if occupants is &gt; 0 it is true</t>
+  </si>
+  <si>
+    <t>If Occupants is &lt; 0 it is true</t>
+  </si>
+  <si>
+    <t>Recognizes if a room is occupied</t>
+  </si>
+  <si>
+    <t>Recognizes if a room is vacant</t>
+  </si>
+  <si>
+    <t>Keeps track of the people in the room</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,7 +199,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -204,7 +233,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -380,19 +408,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="18.28515625" customWidth="1"/>
+    <col min="1" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -406,7 +436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -414,17 +444,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -433,24 +499,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>